<commit_message>
SubsurfaceSinks, ADRE_1DUSS: Fixed volatilization calcs and influent mass allocation
cSubsurfaceSinks - Volatilization was incorrect - had deposition processes as pond-air, and vice-versa. Also had diffusion based on the bulk air, switched to being just gas-phase.

ADRE_1DUSS - Influent mass was misallocated in cases where it went past the first cell. It was being calculated wrong so I changed the calculation to the amount in the first cell will be the ratio of the time to cross the first cell to the total timestep (dt)
</commit_message>
<xml_diff>
--- a/Tracer_test_measurements.xlsx
+++ b/Tracer_test_measurements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SubsurfaceSinks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D2111-6F89-4D2F-90A3-47E3D3C90E32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C58BC9-55E1-4A08-B0CD-A778410388C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0F51068-C0B2-4553-A0D9-69C5A9041677}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Time</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>6PPDQ_meas (ng/L)</t>
+  </si>
+  <si>
+    <t>Rhodamine_meas (mg/L)</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CDBDE2-7098-40D9-8B31-78941A3B2E68}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,9 +426,10 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,13 +442,16 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>0.43055555555555558</v>
+        <v>0.4291666666666667</v>
       </c>
       <c r="B2" s="1">
-        <v>0.75</v>
+        <v>0.71666666673263535</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -452,8 +459,11 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.43124999999999997</v>
       </c>
@@ -466,8 +476,11 @@
       <c r="D3">
         <v>8.9882572725210594E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2.3548773174086999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.43263888888888885</v>
       </c>
@@ -480,8 +493,11 @@
       <c r="D4">
         <v>7.4020708863872992E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0.78744553515667848</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.4368055555555555</v>
       </c>
@@ -494,8 +510,11 @@
       <c r="D5">
         <v>0.1506239168981538</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0.54142822447703309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.44097222222222227</v>
       </c>
@@ -508,8 +527,11 @@
       <c r="D6">
         <v>1.5354037279736938E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0.44704147650757764</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0.44513888888888892</v>
       </c>
@@ -522,8 +544,11 @@
       <c r="D7">
         <v>1.644959623329972E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>0.34435219052229044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0.44791666666666669</v>
       </c>
@@ -536,8 +561,11 @@
       <c r="D8">
         <v>1.6149209935201438E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0.33517570113637113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.4513888888888889</v>
       </c>
@@ -550,8 +578,11 @@
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>0.23336036652117151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0.4548611111111111</v>
       </c>
@@ -564,8 +595,11 @@
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0.26962934837980485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>0.45833333333333331</v>
       </c>
@@ -578,8 +612,11 @@
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>0.17917538157574339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>0.46180555555555558</v>
       </c>
@@ -592,8 +629,11 @@
       <c r="D12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>0.14640220519746025</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>0.46527777777777773</v>
       </c>
@@ -606,8 +646,11 @@
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>0.13460386170127833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0.46875</v>
       </c>
@@ -620,8 +663,11 @@
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>0.12804922642562169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>0.47222222222222199</v>
       </c>
@@ -634,8 +680,11 @@
       <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>0.11537693155935219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>0.47569444444444398</v>
       </c>
@@ -648,8 +697,11 @@
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>0.10314161237812648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>0.47916666666666602</v>
       </c>
@@ -662,8 +714,11 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>0.10051975826786386</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>0.4861111111111111</v>
       </c>
@@ -676,8 +731,11 @@
       <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>0.11144415039395822</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>0.49305555555555602</v>
       </c>
@@ -690,8 +748,11 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>8.1292828125937744E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>0.500000000000001</v>
       </c>
@@ -704,8 +765,11 @@
       <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>7.6486095590456202E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>0.50694444444444597</v>
       </c>
@@ -718,8 +782,11 @@
       <c r="D21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>5.9007068188705193E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>0.51388888888889095</v>
       </c>
@@ -732,8 +799,11 @@
       <c r="D22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>5.3763359968179894E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>0.52083333333333603</v>
       </c>
@@ -746,8 +816,11 @@
       <c r="D23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>6.9931460314799576E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>0.52777777777778201</v>
       </c>
@@ -760,8 +833,11 @@
       <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>5.8570092503661415E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>0.52777777777778201</v>
       </c>
@@ -775,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>0.53472222222222221</v>
       </c>
@@ -788,8 +864,11 @@
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>5.8570092503661415E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -802,8 +881,11 @@
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>5.638521407844254E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>0.54861111111111105</v>
       </c>
@@ -816,8 +898,11 @@
       <c r="D28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>5.201545722800479E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>0.55555555555555503</v>
       </c>
@@ -830,8 +915,11 @@
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>5.201545722800479E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>0.55763888888888891</v>
       </c>
@@ -843,6 +931,9 @@
       </c>
       <c r="D30">
         <v>0</v>
+      </c>
+      <c r="E30">
+        <v>4.5023846267304393E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ModelUpdate: Dmixing (mobile-immobile phase)
Updated the mixing D values so that mixing from mobile to immobile uses mobile phase water Z value, immobile uses immobile phase water. Also ran calibrations - looks like this is pretty OK, potentially, and generated the "synthetic water year" timeseries data (still buggy)
</commit_message>
<xml_diff>
--- a/Tracer_test_measurements.xlsx
+++ b/Tracer_test_measurements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SubsurfaceSinks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C58BC9-55E1-4A08-B0CD-A778410388C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2130A0-B5F5-4DC1-9897-87485D0C6E97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0F51068-C0B2-4553-A0D9-69C5A9041677}"/>
   </bookViews>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>